<commit_message>
Annotated data and analyses and re-added missing DRC data
</commit_message>
<xml_diff>
--- a/1-3-17_cell_invasion_opt_run_2.xlsx
+++ b/1-3-17_cell_invasion_opt_run_2.xlsx
@@ -14,23 +14,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v3.0" hidden="1">Sheet1!$N$2:$N$5</definedName>
-    <definedName name="_xlchart.v3.1" hidden="1">Sheet1!$O$1</definedName>
-    <definedName name="_xlchart.v3.10" hidden="1">Sheet1!$O$3:$O$6</definedName>
-    <definedName name="_xlchart.v3.11" hidden="1">Sheet1!$P$2</definedName>
-    <definedName name="_xlchart.v3.12" hidden="1">Sheet1!$P$3:$P$6</definedName>
-    <definedName name="_xlchart.v3.13" hidden="1">Sheet1!$Q$2</definedName>
-    <definedName name="_xlchart.v3.14" hidden="1">Sheet1!$Q$3:$Q$6</definedName>
-    <definedName name="_xlchart.v3.2" hidden="1">Sheet1!$O$2:$O$5</definedName>
-    <definedName name="_xlchart.v3.3" hidden="1">Sheet1!$P$1</definedName>
-    <definedName name="_xlchart.v3.4" hidden="1">Sheet1!$P$2:$P$5</definedName>
-    <definedName name="_xlchart.v3.5" hidden="1">Sheet1!$Q$1</definedName>
-    <definedName name="_xlchart.v3.6" hidden="1">Sheet1!$Q$2:$Q$5</definedName>
-    <definedName name="_xlchart.v3.7" hidden="1">Sheet1!$Q$2:$Q$5</definedName>
-    <definedName name="_xlchart.v3.8" hidden="1">Sheet1!$N$3:$N$6</definedName>
-    <definedName name="_xlchart.v3.9" hidden="1">Sheet1!$O$2</definedName>
-  </definedNames>
   <calcPr calcId="171027" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Number of colonies</t>
   </si>
@@ -67,6 +50,26 @@
   </si>
   <si>
     <t>Dilution factor</t>
+  </si>
+  <si>
+    <t>Number of colonies * dilution factor</t>
+  </si>
+  <si>
+    <t>Initial colony count</t>
+  </si>
+  <si>
+    <r>
+      <t>Number per 100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>μl * aliquot volume/well volume</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -218,6 +221,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -227,8 +232,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,33 +566,33 @@
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="10"/>
       <c r="M1" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="8"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="10"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
@@ -627,40 +630,40 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="6">
         <v>214</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="6">
         <v>32</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="7">
         <v>3</v>
       </c>
       <c r="H3" s="2">
         <v>1</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="6">
         <v>2140</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="6">
         <v>3200</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="7">
         <v>3000</v>
       </c>
       <c r="N3" s="2">
         <v>1</v>
       </c>
-      <c r="O3" s="9">
-        <f>I3*10</f>
+      <c r="O3" s="6">
+        <f t="shared" ref="O3:Q6" si="0">I3*10</f>
         <v>21400</v>
       </c>
-      <c r="P3" s="9">
-        <f>J3*10</f>
+      <c r="P3" s="6">
+        <f t="shared" si="0"/>
         <v>32000</v>
       </c>
-      <c r="Q3" s="10">
-        <f>K3*10</f>
+      <c r="Q3" s="7">
+        <f t="shared" si="0"/>
         <v>30000</v>
       </c>
     </row>
@@ -668,40 +671,40 @@
       <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="6">
         <v>569</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>83</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="7">
         <v>11</v>
       </c>
       <c r="H4" s="2">
         <v>2</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="6">
         <v>5690</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="6">
         <v>8300</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="7">
         <v>11000</v>
       </c>
       <c r="N4" s="2">
         <v>2</v>
       </c>
-      <c r="O4" s="9">
-        <f>I4*10</f>
+      <c r="O4" s="6">
+        <f t="shared" si="0"/>
         <v>56900</v>
       </c>
-      <c r="P4" s="9">
-        <f>J4*10</f>
+      <c r="P4" s="6">
+        <f t="shared" si="0"/>
         <v>83000</v>
       </c>
-      <c r="Q4" s="10">
-        <f>K4*10</f>
+      <c r="Q4" s="7">
+        <f t="shared" si="0"/>
         <v>110000</v>
       </c>
     </row>
@@ -709,40 +712,40 @@
       <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="6">
         <v>897</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>118</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="7">
         <v>14</v>
       </c>
       <c r="H5" s="2">
         <v>3</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="6">
         <v>8970</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="6">
         <v>11800</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="7">
         <v>14000</v>
       </c>
       <c r="N5" s="2">
         <v>3</v>
       </c>
-      <c r="O5" s="9">
-        <f>I5*10</f>
+      <c r="O5" s="6">
+        <f t="shared" si="0"/>
         <v>89700</v>
       </c>
-      <c r="P5" s="9">
-        <f>J5*10</f>
+      <c r="P5" s="6">
+        <f t="shared" si="0"/>
         <v>118000</v>
       </c>
-      <c r="Q5" s="10">
-        <f>K5*10</f>
+      <c r="Q5" s="7">
+        <f t="shared" si="0"/>
         <v>140000</v>
       </c>
     </row>
@@ -775,16 +778,27 @@
         <v>4</v>
       </c>
       <c r="O6" s="4">
-        <f>I6*10</f>
+        <f t="shared" si="0"/>
         <v>37000</v>
       </c>
       <c r="P6" s="4">
-        <f>J6*10</f>
+        <f t="shared" si="0"/>
         <v>75000</v>
       </c>
       <c r="Q6" s="5">
-        <f>K6*10</f>
+        <f t="shared" si="0"/>
         <v>110000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>